<commit_message>
added more wines to weinbar
</commit_message>
<xml_diff>
--- a/Weinbar.xlsx
+++ b/Weinbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_f70\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527EA21-5FA2-5541-9C06-1883B909B780}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED99DEC2-F667-884A-9BAC-EFB312428905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="383">
   <si>
     <t>name</t>
   </si>
@@ -1151,10 +1151,25 @@
     <t>Barriton</t>
   </si>
   <si>
+    <t>Marani</t>
+  </si>
+  <si>
     <t>Marani Tvishi</t>
   </si>
   <si>
-    <t>suess, herb, sueffig</t>
+    <t>Tsolikauri</t>
+  </si>
+  <si>
+    <t>Racha-Lechkhumi</t>
+  </si>
+  <si>
+    <t>suess, herb, sueffig, banane</t>
+  </si>
+  <si>
+    <t>nelken, schwer, zimt, flach, bitter</t>
+  </si>
+  <si>
+    <t>Michel Schneider</t>
   </si>
 </sst>
 </file>
@@ -1995,13 +2010,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M113"/>
+  <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.9140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -5862,7 +5880,10 @@
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>373</v>
+        <v>374</v>
+      </c>
+      <c r="B113" t="s">
+        <v>375</v>
       </c>
       <c r="C113" t="s">
         <v>146</v>
@@ -5870,8 +5891,17 @@
       <c r="D113" t="s">
         <v>319</v>
       </c>
+      <c r="E113" t="s">
+        <v>376</v>
+      </c>
+      <c r="F113" t="s">
+        <v>373</v>
+      </c>
       <c r="G113" t="s">
-        <v>374</v>
+        <v>377</v>
+      </c>
+      <c r="I113">
+        <v>11</v>
       </c>
       <c r="J113">
         <v>11.5</v>
@@ -5884,6 +5914,47 @@
       </c>
       <c r="M113" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>45</v>
+      </c>
+      <c r="B114" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" t="s">
+        <v>15</v>
+      </c>
+      <c r="D114" t="s">
+        <v>119</v>
+      </c>
+      <c r="E114" t="s">
+        <v>155</v>
+      </c>
+      <c r="F114" t="s">
+        <v>379</v>
+      </c>
+      <c r="G114" t="s">
+        <v>378</v>
+      </c>
+      <c r="H114" t="s">
+        <v>53</v>
+      </c>
+      <c r="I114">
+        <v>12</v>
+      </c>
+      <c r="J114">
+        <v>1.99</v>
+      </c>
+      <c r="K114">
+        <v>2019</v>
+      </c>
+      <c r="L114" t="s">
+        <v>21</v>
+      </c>
+      <c r="M114" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added onemore wine to weinbar
</commit_message>
<xml_diff>
--- a/Weinbar.xlsx
+++ b/Weinbar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_f70\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED99DEC2-F667-884A-9BAC-EFB312428905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC07B7E4-C660-0642-B6CF-75820CC53F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="386">
   <si>
     <t>name</t>
   </si>
@@ -1170,13 +1170,28 @@
   </si>
   <si>
     <t>Michel Schneider</t>
+  </si>
+  <si>
+    <t>Tierra de Castilla Rosado</t>
+  </si>
+  <si>
+    <t>Denns</t>
+  </si>
+  <si>
+    <t>honig, flieder, wuerzig</t>
+  </si>
+  <si>
+    <t>La Mancha</t>
+  </si>
+  <si>
+    <t>Oekoweine Haus am Goldberg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1310,6 +1325,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto-Light"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1653,8 +1674,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2010,15 +2034,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M114"/>
+  <dimension ref="A1:M115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="F114" sqref="F114"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.8671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -5957,6 +5982,47 @@
         <v>20</v>
       </c>
     </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>380</v>
+      </c>
+      <c r="B115" t="s">
+        <v>93</v>
+      </c>
+      <c r="C115" t="s">
+        <v>131</v>
+      </c>
+      <c r="D115" t="s">
+        <v>43</v>
+      </c>
+      <c r="E115" t="s">
+        <v>383</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="G115" t="s">
+        <v>382</v>
+      </c>
+      <c r="H115" t="s">
+        <v>381</v>
+      </c>
+      <c r="I115">
+        <v>13</v>
+      </c>
+      <c r="J115">
+        <v>6</v>
+      </c>
+      <c r="K115">
+        <v>2019</v>
+      </c>
+      <c r="L115" t="s">
+        <v>21</v>
+      </c>
+      <c r="M115" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added 1112 and freixenet
</commit_message>
<xml_diff>
--- a/Weinbar.xlsx
+++ b/Weinbar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_f70\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juliana Schneider\dev\Weinbar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC07B7E4-C660-0642-B6CF-75820CC53F20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C8902C-3217-43EA-B3E9-CBE13C6D85BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="390">
   <si>
     <t>name</t>
   </si>
@@ -1028,9 +1028,6 @@
     <t>leicht, spritzig, frisch, saeuerlich</t>
   </si>
   <si>
-    <t>112 Blanc de Noirs</t>
-  </si>
-  <si>
     <t>Markgraeflich Badisches Weinhaus</t>
   </si>
   <si>
@@ -1185,13 +1182,31 @@
   </si>
   <si>
     <t>Oekoweine Haus am Goldberg</t>
+  </si>
+  <si>
+    <t>1112 Blanc de Noirs</t>
+  </si>
+  <si>
+    <t>1112 Grauburgunder</t>
+  </si>
+  <si>
+    <t>Freixenet Carta Rose Dry</t>
+  </si>
+  <si>
+    <t>Garnacha, Trepat</t>
+  </si>
+  <si>
+    <t>Cava</t>
+  </si>
+  <si>
+    <t>Henkell-Freixenet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2034,19 +2049,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M115"/>
+  <dimension ref="A1:M117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="N117" sqref="N117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.8671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2087,7 +2102,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2119,7 +2134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2157,7 +2172,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -2195,7 +2210,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2233,7 +2248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2256,7 +2271,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -2285,7 +2300,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -2311,7 +2326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -2349,7 +2364,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -2384,7 +2399,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -2419,7 +2434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -2454,7 +2469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2489,7 +2504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13">
       <c r="A14" t="s">
         <v>66</v>
       </c>
@@ -2515,7 +2530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13">
       <c r="A15" t="s">
         <v>71</v>
       </c>
@@ -2556,7 +2571,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13">
       <c r="A16" t="s">
         <v>73</v>
       </c>
@@ -2594,7 +2609,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2635,7 +2650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -2658,7 +2673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2696,7 +2711,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2719,7 +2734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -2742,7 +2757,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2765,7 +2780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -2785,7 +2800,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2805,7 +2820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2831,7 +2846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>101</v>
       </c>
@@ -2857,7 +2872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>103</v>
       </c>
@@ -2880,7 +2895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>105</v>
       </c>
@@ -2906,7 +2921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -2923,7 +2938,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -2946,7 +2961,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -2972,7 +2987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -3004,7 +3019,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13">
       <c r="A33" t="s">
         <v>118</v>
       </c>
@@ -3039,7 +3054,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -3080,7 +3095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13">
       <c r="A35" t="s">
         <v>129</v>
       </c>
@@ -3109,7 +3124,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13">
       <c r="A36" t="s">
         <v>135</v>
       </c>
@@ -3150,7 +3165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13">
       <c r="A37" t="s">
         <v>142</v>
       </c>
@@ -3185,7 +3200,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13">
       <c r="A38" t="s">
         <v>143</v>
       </c>
@@ -3220,7 +3235,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13">
       <c r="A39" t="s">
         <v>144</v>
       </c>
@@ -3255,7 +3270,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -3287,7 +3302,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13">
       <c r="A41" t="s">
         <v>148</v>
       </c>
@@ -3319,7 +3334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -3351,7 +3366,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13">
       <c r="A43" t="s">
         <v>152</v>
       </c>
@@ -3380,7 +3395,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13">
       <c r="A44" t="s">
         <v>154</v>
       </c>
@@ -3409,7 +3424,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13">
       <c r="B45" t="s">
         <v>157</v>
       </c>
@@ -3435,7 +3450,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13">
       <c r="A46" t="s">
         <v>159</v>
       </c>
@@ -3467,7 +3482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13">
       <c r="A47" t="s">
         <v>163</v>
       </c>
@@ -3505,7 +3520,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13">
       <c r="A48" t="s">
         <v>165</v>
       </c>
@@ -3534,7 +3549,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13">
       <c r="A49" t="s">
         <v>168</v>
       </c>
@@ -3563,7 +3578,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13">
       <c r="A50" t="s">
         <v>152</v>
       </c>
@@ -3598,7 +3613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13">
       <c r="A51" t="s">
         <v>152</v>
       </c>
@@ -3627,7 +3642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13">
       <c r="A52" t="s">
         <v>175</v>
       </c>
@@ -3665,7 +3680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13">
       <c r="A53" t="s">
         <v>177</v>
       </c>
@@ -3697,7 +3712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13">
       <c r="A54" t="s">
         <v>180</v>
       </c>
@@ -3738,7 +3753,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13">
       <c r="A55" t="s">
         <v>183</v>
       </c>
@@ -3773,7 +3788,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13">
       <c r="A56" t="s">
         <v>187</v>
       </c>
@@ -3805,7 +3820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13">
       <c r="A57" t="s">
         <v>192</v>
       </c>
@@ -3843,7 +3858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13">
       <c r="A58" t="s">
         <v>79</v>
       </c>
@@ -3884,7 +3899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13">
       <c r="A59" t="s">
         <v>196</v>
       </c>
@@ -3919,7 +3934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13">
       <c r="A60" t="s">
         <v>198</v>
       </c>
@@ -3954,7 +3969,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13">
       <c r="A61" t="s">
         <v>203</v>
       </c>
@@ -3980,7 +3995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13">
       <c r="A62" t="s">
         <v>199</v>
       </c>
@@ -4006,7 +4021,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13">
       <c r="A63" t="s">
         <v>206</v>
       </c>
@@ -4029,7 +4044,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13">
       <c r="A64" t="s">
         <v>154</v>
       </c>
@@ -4055,7 +4070,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13">
       <c r="A65" t="s">
         <v>208</v>
       </c>
@@ -4078,7 +4093,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13">
       <c r="A66" t="s">
         <v>209</v>
       </c>
@@ -4104,7 +4119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13">
       <c r="A67" t="s">
         <v>211</v>
       </c>
@@ -4136,7 +4151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13">
       <c r="A68" t="s">
         <v>215</v>
       </c>
@@ -4168,7 +4183,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13">
       <c r="A69" t="s">
         <v>219</v>
       </c>
@@ -4209,7 +4224,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13">
       <c r="A70" t="s">
         <v>223</v>
       </c>
@@ -4250,7 +4265,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13">
       <c r="A71" t="s">
         <v>228</v>
       </c>
@@ -4288,7 +4303,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13">
       <c r="A72" t="s">
         <v>231</v>
       </c>
@@ -4329,7 +4344,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13">
       <c r="A73" t="s">
         <v>236</v>
       </c>
@@ -4370,7 +4385,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13">
       <c r="A74" t="s">
         <v>239</v>
       </c>
@@ -4408,7 +4423,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13">
       <c r="A75" t="s">
         <v>242</v>
       </c>
@@ -4446,7 +4461,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13">
       <c r="A76" t="s">
         <v>244</v>
       </c>
@@ -4484,7 +4499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13">
       <c r="A77" t="s">
         <v>247</v>
       </c>
@@ -4516,7 +4531,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13">
       <c r="A78" t="s">
         <v>251</v>
       </c>
@@ -4557,7 +4572,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13">
       <c r="A79" t="s">
         <v>255</v>
       </c>
@@ -4598,7 +4613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13">
       <c r="A80" t="s">
         <v>258</v>
       </c>
@@ -4639,7 +4654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" t="s">
         <v>263</v>
       </c>
@@ -4677,7 +4692,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82" t="s">
         <v>269</v>
       </c>
@@ -4718,7 +4733,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83" t="s">
         <v>274</v>
       </c>
@@ -4756,7 +4771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84" t="s">
         <v>278</v>
       </c>
@@ -4797,7 +4812,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85" t="s">
         <v>282</v>
       </c>
@@ -4838,7 +4853,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86" t="s">
         <v>285</v>
       </c>
@@ -4879,7 +4894,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87" t="s">
         <v>288</v>
       </c>
@@ -4920,7 +4935,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13">
       <c r="A88" t="s">
         <v>293</v>
       </c>
@@ -4955,7 +4970,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13">
       <c r="A89" t="s">
         <v>296</v>
       </c>
@@ -4993,7 +5008,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13">
       <c r="A90" t="s">
         <v>300</v>
       </c>
@@ -5031,7 +5046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13">
       <c r="A91" t="s">
         <v>302</v>
       </c>
@@ -5069,7 +5084,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13">
       <c r="A92" t="s">
         <v>306</v>
       </c>
@@ -5110,7 +5125,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13">
       <c r="A93" t="s">
         <v>39</v>
       </c>
@@ -5151,7 +5166,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13">
       <c r="A94" t="s">
         <v>309</v>
       </c>
@@ -5186,7 +5201,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -5227,7 +5242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13">
       <c r="A96" t="s">
         <v>317</v>
       </c>
@@ -5262,7 +5277,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13">
       <c r="A97" t="s">
         <v>323</v>
       </c>
@@ -5297,7 +5312,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13">
       <c r="A98" t="s">
         <v>327</v>
       </c>
@@ -5338,7 +5353,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13">
       <c r="A99" t="s">
         <v>329</v>
       </c>
@@ -5376,9 +5391,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13">
       <c r="A100" t="s">
-        <v>332</v>
+        <v>384</v>
       </c>
       <c r="B100" t="s">
         <v>275</v>
@@ -5393,10 +5408,10 @@
         <v>161</v>
       </c>
       <c r="F100" t="s">
+        <v>332</v>
+      </c>
+      <c r="G100" t="s">
         <v>333</v>
-      </c>
-      <c r="G100" t="s">
-        <v>334</v>
       </c>
       <c r="I100">
         <v>12.5</v>
@@ -5414,7 +5429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13">
       <c r="A101" t="s">
         <v>152</v>
       </c>
@@ -5425,16 +5440,16 @@
         <v>146</v>
       </c>
       <c r="D101" t="s">
+        <v>334</v>
+      </c>
+      <c r="E101" t="s">
         <v>335</v>
-      </c>
-      <c r="E101" t="s">
-        <v>336</v>
       </c>
       <c r="F101" t="s">
         <v>182</v>
       </c>
       <c r="G101" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H101" t="s">
         <v>78</v>
@@ -5455,12 +5470,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13">
       <c r="A102" t="s">
+        <v>337</v>
+      </c>
+      <c r="B102" t="s">
         <v>338</v>
-      </c>
-      <c r="B102" t="s">
-        <v>339</v>
       </c>
       <c r="C102" t="s">
         <v>15</v>
@@ -5472,10 +5487,10 @@
         <v>252</v>
       </c>
       <c r="F102" t="s">
+        <v>339</v>
+      </c>
+      <c r="G102" t="s">
         <v>340</v>
-      </c>
-      <c r="G102" t="s">
-        <v>341</v>
       </c>
       <c r="H102" t="s">
         <v>87</v>
@@ -5496,9 +5511,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13">
       <c r="A103" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -5513,10 +5528,10 @@
         <v>161</v>
       </c>
       <c r="F103" t="s">
+        <v>342</v>
+      </c>
+      <c r="G103" t="s">
         <v>343</v>
-      </c>
-      <c r="G103" t="s">
-        <v>344</v>
       </c>
       <c r="H103" t="s">
         <v>53</v>
@@ -5537,12 +5552,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13">
       <c r="A104" t="s">
+        <v>344</v>
+      </c>
+      <c r="B104" t="s">
         <v>345</v>
-      </c>
-      <c r="B104" t="s">
-        <v>346</v>
       </c>
       <c r="C104" t="s">
         <v>146</v>
@@ -5554,10 +5569,10 @@
         <v>173</v>
       </c>
       <c r="F104" t="s">
+        <v>346</v>
+      </c>
+      <c r="G104" t="s">
         <v>347</v>
-      </c>
-      <c r="G104" t="s">
-        <v>348</v>
       </c>
       <c r="H104" t="s">
         <v>78</v>
@@ -5578,7 +5593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13">
       <c r="A105" t="s">
         <v>180</v>
       </c>
@@ -5598,7 +5613,7 @@
         <v>182</v>
       </c>
       <c r="G105" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H105" t="s">
         <v>78</v>
@@ -5619,9 +5634,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13">
       <c r="A106" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B106" t="s">
         <v>206</v>
@@ -5639,7 +5654,7 @@
         <v>304</v>
       </c>
       <c r="G106" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H106" t="s">
         <v>87</v>
@@ -5660,9 +5675,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13">
       <c r="A107" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B107" t="s">
         <v>164</v>
@@ -5677,7 +5692,7 @@
         <v>161</v>
       </c>
       <c r="F107" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G107" t="s">
         <v>328</v>
@@ -5701,9 +5716,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13">
       <c r="A108" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B108" t="s">
         <v>275</v>
@@ -5718,10 +5733,10 @@
         <v>161</v>
       </c>
       <c r="F108" t="s">
+        <v>354</v>
+      </c>
+      <c r="G108" t="s">
         <v>355</v>
-      </c>
-      <c r="G108" t="s">
-        <v>356</v>
       </c>
       <c r="H108" t="s">
         <v>78</v>
@@ -5742,9 +5757,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13">
       <c r="A109" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B109" t="s">
         <v>199</v>
@@ -5759,10 +5774,10 @@
         <v>200</v>
       </c>
       <c r="F109" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G109" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H109" t="s">
         <v>19</v>
@@ -5783,12 +5798,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13">
       <c r="A110" t="s">
+        <v>359</v>
+      </c>
+      <c r="B110" t="s">
         <v>360</v>
-      </c>
-      <c r="B110" t="s">
-        <v>361</v>
       </c>
       <c r="C110" t="s">
         <v>131</v>
@@ -5797,16 +5812,16 @@
         <v>43</v>
       </c>
       <c r="E110" t="s">
+        <v>361</v>
+      </c>
+      <c r="F110" t="s">
         <v>362</v>
       </c>
-      <c r="F110" t="s">
+      <c r="G110" t="s">
         <v>363</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>364</v>
-      </c>
-      <c r="H110" t="s">
-        <v>365</v>
       </c>
       <c r="I110">
         <v>13.5</v>
@@ -5824,9 +5839,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13">
       <c r="A111" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B111" t="s">
         <v>224</v>
@@ -5841,13 +5856,13 @@
         <v>225</v>
       </c>
       <c r="F111" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G111" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H111" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I111">
         <v>12.5</v>
@@ -5865,9 +5880,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13">
       <c r="A112" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B112" t="s">
         <v>93</v>
@@ -5879,13 +5894,13 @@
         <v>43</v>
       </c>
       <c r="E112" t="s">
+        <v>369</v>
+      </c>
+      <c r="F112" t="s">
+        <v>371</v>
+      </c>
+      <c r="G112" t="s">
         <v>370</v>
-      </c>
-      <c r="F112" t="s">
-        <v>372</v>
-      </c>
-      <c r="G112" t="s">
-        <v>371</v>
       </c>
       <c r="I112">
         <v>13.5</v>
@@ -5903,12 +5918,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13">
       <c r="A113" t="s">
+        <v>373</v>
+      </c>
+      <c r="B113" t="s">
         <v>374</v>
-      </c>
-      <c r="B113" t="s">
-        <v>375</v>
       </c>
       <c r="C113" t="s">
         <v>146</v>
@@ -5917,13 +5932,13 @@
         <v>319</v>
       </c>
       <c r="E113" t="s">
+        <v>375</v>
+      </c>
+      <c r="F113" t="s">
+        <v>372</v>
+      </c>
+      <c r="G113" t="s">
         <v>376</v>
-      </c>
-      <c r="F113" t="s">
-        <v>373</v>
-      </c>
-      <c r="G113" t="s">
-        <v>377</v>
       </c>
       <c r="I113">
         <v>11</v>
@@ -5941,7 +5956,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13">
       <c r="A114" t="s">
         <v>45</v>
       </c>
@@ -5958,10 +5973,10 @@
         <v>155</v>
       </c>
       <c r="F114" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="G114" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H114" t="s">
         <v>53</v>
@@ -5982,9 +5997,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="24.75">
       <c r="A115" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B115" t="s">
         <v>93</v>
@@ -5996,16 +6011,16 @@
         <v>43</v>
       </c>
       <c r="E115" t="s">
+        <v>382</v>
+      </c>
+      <c r="F115" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="F115" s="1" t="s">
-        <v>384</v>
-      </c>
       <c r="G115" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H115" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I115">
         <v>13</v>
@@ -6020,6 +6035,88 @@
         <v>21</v>
       </c>
       <c r="M115" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13">
+      <c r="A116" t="s">
+        <v>385</v>
+      </c>
+      <c r="B116" t="s">
+        <v>145</v>
+      </c>
+      <c r="C116" t="s">
+        <v>146</v>
+      </c>
+      <c r="D116" t="s">
+        <v>119</v>
+      </c>
+      <c r="E116" t="s">
+        <v>161</v>
+      </c>
+      <c r="F116" t="s">
+        <v>332</v>
+      </c>
+      <c r="G116" t="s">
+        <v>202</v>
+      </c>
+      <c r="H116" t="s">
+        <v>87</v>
+      </c>
+      <c r="I116">
+        <v>13</v>
+      </c>
+      <c r="J116">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K116">
+        <v>2019</v>
+      </c>
+      <c r="L116" t="s">
+        <v>21</v>
+      </c>
+      <c r="M116" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13">
+      <c r="A117" t="s">
+        <v>386</v>
+      </c>
+      <c r="B117" t="s">
+        <v>387</v>
+      </c>
+      <c r="C117" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" t="s">
+        <v>43</v>
+      </c>
+      <c r="E117" t="s">
+        <v>388</v>
+      </c>
+      <c r="F117" t="s">
+        <v>389</v>
+      </c>
+      <c r="G117" t="s">
+        <v>47</v>
+      </c>
+      <c r="H117" t="s">
+        <v>87</v>
+      </c>
+      <c r="I117">
+        <v>12</v>
+      </c>
+      <c r="J117">
+        <v>5.99</v>
+      </c>
+      <c r="K117">
+        <v>2019</v>
+      </c>
+      <c r="L117" t="s">
+        <v>21</v>
+      </c>
+      <c r="M117" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>